<commit_message>
v0.2 - opens and scrapes needed metadata to excel
</commit_message>
<xml_diff>
--- a/xlsx/urls.xlsx
+++ b/xlsx/urls.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\root\workspace\github.com\RimvydasZ\Google-PlayStore-Metadata-to-Excel\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rimvy\dev\Google-PlayStore-Metadata-to-Excel\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618B11CE-098F-4EF3-B2D6-0B2136711C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3C1BF7-2DF9-44F0-818E-229706D24144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4965" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>https://play.google.com/store/apps/details?id=com.busegame.bilgelik</t>
   </si>
@@ -34,24 +34,6 @@
   </si>
   <si>
     <t>https://play.google.com/store/apps/details?id=com.appone.radio.norge</t>
-  </si>
-  <si>
-    <t>https://play.google.com/store/apps/details?id=com.zagyapps.linafootligue1</t>
-  </si>
-  <si>
-    <t>https://play.google.com/store/apps/details?id=com.alexto.radiosdemexicoonlinegratis</t>
-  </si>
-  <si>
-    <t>https://play.google.com/store/apps/details?id=com.appone.radio.USA</t>
-  </si>
-  <si>
-    <t>https://play.google.com/store/apps/details?id=net.telewebion</t>
-  </si>
-  <si>
-    <t>https://play.google.com/store/apps/details?id=com.peemz.fanions</t>
-  </si>
-  <si>
-    <t>https://play.google.com/store/apps/details?id=com.appone.radios.ireland.fm</t>
   </si>
   <si>
     <t>https://play.google.com/store/apps/details?id=com.matteljv.uno</t>
@@ -375,17 +357,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -406,36 +388,6 @@
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>